<commit_message>
Edited README. Changed class names.
</commit_message>
<xml_diff>
--- a/logs/BettingInformation.xlsx
+++ b/logs/BettingInformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>Time</t>
   </si>
@@ -29,9 +29,6 @@
     <t>Prediction</t>
   </si>
   <si>
-    <t>Score prediction</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Odds Home Win</t>
   </si>
   <si>
@@ -41,28 +38,67 @@
     <t>Odds Away Win</t>
   </si>
   <si>
-    <t>16:00</t>
-  </si>
-  <si>
-    <t>Kuktosh - Khujand</t>
-  </si>
-  <si>
-    <t>Vysshaya Liga</t>
-  </si>
-  <si>
-    <t>Away</t>
-  </si>
-  <si>
-    <t>0 - 1</t>
-  </si>
-  <si>
-    <t>5.22</t>
-  </si>
-  <si>
-    <t>4.45</t>
-  </si>
-  <si>
-    <t>1.47</t>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>Pho Hien (Vie) - Nam Dinh (Vie)</t>
+  </si>
+  <si>
+    <t>Club Friendly</t>
+  </si>
+  <si>
+    <t>H 2 - 1</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>1.89</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>Shakhtyor Soligorsk - Brest</t>
+  </si>
+  <si>
+    <t>Belarusian Cup</t>
+  </si>
+  <si>
+    <t>Home 2 - 0</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>BATE - Slavia Mozyr</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>Esteli - Diriangen</t>
+  </si>
+  <si>
+    <t>Liga Primera</t>
+  </si>
+  <si>
+    <t>H 1 - 0</t>
+  </si>
+  <si>
+    <t>2.34</t>
   </si>
 </sst>
 </file>
@@ -184,20 +220,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.21484375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="21.12109375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.44921875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.47265625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.51171875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.95703125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="10.15625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="14.95703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.15625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -222,34 +257,97 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -259,7 +357,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -287,9 +385,6 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -298,7 +393,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -326,9 +421,6 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -337,7 +429,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -365,9 +457,6 @@
       <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Soccer info parser fixed, generalized to scrap data of all event that are present
</commit_message>
<xml_diff>
--- a/logs/BettingInformation.xlsx
+++ b/logs/BettingInformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Time</t>
   </si>
@@ -38,6 +38,63 @@
     <t>Odds Away Win</t>
   </si>
   <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>Shakhtyor Soligorsk - Brest</t>
+  </si>
+  <si>
+    <t>Belarusian Cup</t>
+  </si>
+  <si>
+    <t>Home 2 - 0</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t>3.38</t>
+  </si>
+  <si>
+    <t>3.96</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>BATE - Slavia Mozyr</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>4.94</t>
+  </si>
+  <si>
+    <t>9.13</t>
+  </si>
+  <si>
+    <t>23:00</t>
+  </si>
+  <si>
+    <t>Esteli - Diriangen</t>
+  </si>
+  <si>
+    <t>Liga Primera</t>
+  </si>
+  <si>
+    <t>H 1 - 0</t>
+  </si>
+  <si>
+    <t>2.34</t>
+  </si>
+  <si>
+    <t>2.75</t>
+  </si>
+  <si>
+    <t>3.28</t>
+  </si>
+  <si>
     <t>11:00</t>
   </si>
   <si>
@@ -57,48 +114,6 @@
   </si>
   <si>
     <t>1.89</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>Shakhtyor Soligorsk - Brest</t>
-  </si>
-  <si>
-    <t>Belarusian Cup</t>
-  </si>
-  <si>
-    <t>Home 2 - 0</t>
-  </si>
-  <si>
-    <t>1.92</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>20:00</t>
-  </si>
-  <si>
-    <t>BATE - Slavia Mozyr</t>
-  </si>
-  <si>
-    <t>1.32</t>
-  </si>
-  <si>
-    <t>23:00</t>
-  </si>
-  <si>
-    <t>Esteli - Diriangen</t>
-  </si>
-  <si>
-    <t>Liga Primera</t>
-  </si>
-  <si>
-    <t>H 1 - 0</t>
-  </si>
-  <si>
-    <t>2.34</t>
   </si>
 </sst>
 </file>
@@ -289,65 +304,65 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>